<commit_message>
State 4 Test Plan
State 4 Test Plan
</commit_message>
<xml_diff>
--- a/documentation/Test Plan.xlsx
+++ b/documentation/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SERVERMS30\usuarios$\secundaria\nicolas.philippe\Documents\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E9926-DEFA-4DE6-8CE6-79D39657E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DD7F06-5EA0-4F54-9A17-DE70A01B4C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D0778657-FC13-4815-9E31-E63064B32010}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="105">
   <si>
     <t>Test Plan</t>
   </si>
@@ -53,6 +53,156 @@
     <t>Expected Output</t>
   </si>
   <si>
+    <t>Criteria A</t>
+  </si>
+  <si>
+    <t>Verify implementation of Tic Tac Toe and Checkers</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Both games are available and functional within the application</t>
+  </si>
+  <si>
+    <t>Criteria B</t>
+  </si>
+  <si>
+    <t>Ensure both players can play in the same Java application</t>
+  </si>
+  <si>
+    <t>Both players can play without remote connections</t>
+  </si>
+  <si>
+    <t>Criteria C</t>
+  </si>
+  <si>
+    <t>Test game selection functionality</t>
+  </si>
+  <si>
+    <t>Select Tic Tac Toe, Select Checkers</t>
+  </si>
+  <si>
+    <t>Correct game is launched based on player selection</t>
+  </si>
+  <si>
+    <t>Criteria D</t>
+  </si>
+  <si>
+    <t>Test player name management</t>
+  </si>
+  <si>
+    <t>Create, select, correct, delete names</t>
+  </si>
+  <si>
+    <t>Player names are managed correctly (created, selected, corrected, deleted)</t>
+  </si>
+  <si>
+    <t>Criteria E</t>
+  </si>
+  <si>
+    <t>Verify display of game boards, player names, and turns</t>
+  </si>
+  <si>
+    <t>Game boards, player names, and turns are displayed clearly</t>
+  </si>
+  <si>
+    <t>Criteria F</t>
+  </si>
+  <si>
+    <t>Test score and ranking updates</t>
+  </si>
+  <si>
+    <t>Play games, check scores and rankings</t>
+  </si>
+  <si>
+    <t>Scores and rankings are updated and displayed correctly before and after games</t>
+  </si>
+  <si>
+    <t>Criteria G</t>
+  </si>
+  <si>
+    <t>Test penalty for canceling a mid-play game</t>
+  </si>
+  <si>
+    <t>Cancel game mid-play</t>
+  </si>
+  <si>
+    <t>Players are penalized appropriately for canceling mid-play</t>
+  </si>
+  <si>
+    <t>Detailed Test Cases</t>
+  </si>
+  <si>
+    <t>Criteria A: Implement two games: Tic Tac Toe and Checkers</t>
+  </si>
+  <si>
+    <t>Verify Tic Tac Toe implementation</t>
+  </si>
+  <si>
+    <t>Verify Checkers implementation</t>
+  </si>
+  <si>
+    <t>Criteria B: Players are playing in the same Java application (no remote)</t>
+  </si>
+  <si>
+    <t>Ensure both players can play in the same application</t>
+  </si>
+  <si>
+    <t>Criteria C: Allow players to choose which game to play</t>
+  </si>
+  <si>
+    <t>Criteria D: Manage player name, including creation, selection, correction, and deletion</t>
+  </si>
+  <si>
+    <t>Create player name</t>
+  </si>
+  <si>
+    <t>"Player1"</t>
+  </si>
+  <si>
+    <t>Player name "Player1" is created</t>
+  </si>
+  <si>
+    <t>Select player name</t>
+  </si>
+  <si>
+    <t>Player name "Player1" is selected</t>
+  </si>
+  <si>
+    <t>Player name is updated to "PlayerOne"</t>
+  </si>
+  <si>
+    <t>Criteria E: Display game boards, player names, and turns clearly</t>
+  </si>
+  <si>
+    <t>Verify display of game boards</t>
+  </si>
+  <si>
+    <t>Game boards are displayed clearly</t>
+  </si>
+  <si>
+    <t>Verify display of player names</t>
+  </si>
+  <si>
+    <t>Player names are displayed clearly</t>
+  </si>
+  <si>
+    <t>Verify display of turns</t>
+  </si>
+  <si>
+    <t>Turns are displayed clearly</t>
+  </si>
+  <si>
+    <t>Criteria F: Update and display scores and rankings after and before each game</t>
+  </si>
+  <si>
+    <t>Play Tic Tac Toe, Checkers</t>
+  </si>
+  <si>
+    <t>Criteria G: Penalize players for canceling a mid-play game</t>
+  </si>
+  <si>
     <t>Data Types</t>
   </si>
   <si>
@@ -62,13 +212,145 @@
     <t>Extreme Data</t>
   </si>
   <si>
+    <t>"A very very long player name"</t>
+  </si>
+  <si>
+    <t>Player name is created or appropriate error message is displayed</t>
+  </si>
+  <si>
+    <t>Play multiple games</t>
+  </si>
+  <si>
+    <t>Play 100 games</t>
+  </si>
+  <si>
+    <t>Scores and rankings are updated correctly</t>
+  </si>
+  <si>
     <t>Erroneous Data</t>
   </si>
   <si>
-    <t>Detailed Test Cases For Each Sucess Criteroa</t>
-  </si>
-  <si>
-    <t>Success Criteria XXX</t>
+    <t>"" (empty string)</t>
+  </si>
+  <si>
+    <t>Appropriate error message is displayed</t>
+  </si>
+  <si>
+    <t>Add end of each game, navigate to result view</t>
+  </si>
+  <si>
+    <t>Result View is Launched at end of game</t>
+  </si>
+  <si>
+    <t>Tic Tac Toe game is available and functional: check player turns, move validation, game termination, board actualization at each turn</t>
+  </si>
+  <si>
+    <t>Checkers game is available and functional: check player turns, move validation, game termination, board actualization at each turn</t>
+  </si>
+  <si>
+    <t>Player selection View is Launched</t>
+  </si>
+  <si>
+    <t>Click start game</t>
+  </si>
+  <si>
+    <t>The selected game is started</t>
+  </si>
+  <si>
+    <t>Once two players are successfully selected on Player Selection View</t>
+  </si>
+  <si>
+    <t>Select Checkers on Game Selection view</t>
+  </si>
+  <si>
+    <t>Select Tic Tac Toe on Game Selection view</t>
+  </si>
+  <si>
+    <t>Launch Change Name View</t>
+  </si>
+  <si>
+    <t>Launch Create Name View</t>
+  </si>
+  <si>
+    <t>Player name "Player1" is created, saved in DB, and when returning to Player Selection View it is Selected in the Player 1/2 field</t>
+  </si>
+  <si>
+    <t>Launch Player Selection View from Tic Tac Toe</t>
+  </si>
+  <si>
+    <t>Launch Player Selection View from Checkers</t>
+  </si>
+  <si>
+    <t>Launch manage names</t>
+  </si>
+  <si>
+    <t>Launch new for Player 1 or Player 2</t>
+  </si>
+  <si>
+    <t>In Player Selection View, select manage names</t>
+  </si>
+  <si>
+    <t>In Player Selection View select new for player 1 or 2</t>
+  </si>
+  <si>
+    <t>In create Player View , create a "Player1" name and accept</t>
+  </si>
+  <si>
+    <t>Create player name and cancel</t>
+  </si>
+  <si>
+    <t>In create Player View , create a "Player1" name and cancel</t>
+  </si>
+  <si>
+    <t>Return Player Selection with no change</t>
+  </si>
+  <si>
+    <t>Create valid player name and accept</t>
+  </si>
+  <si>
+    <t>Create duplicate player name and accept</t>
+  </si>
+  <si>
+    <t>In create Player View , create a duplicate "Player1" name and accept</t>
+  </si>
+  <si>
+    <t>error message is shown, and back to same view</t>
+  </si>
+  <si>
+    <t>Correct player name and cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no change, and return to Player Selection View </t>
+  </si>
+  <si>
+    <t>Correct player name and accept</t>
+  </si>
+  <si>
+    <t>In Manage Playe Namer View "Player1" to "PlayerOne" and cancel</t>
+  </si>
+  <si>
+    <t>In Manage Playe Namer View "Player1" to "PlayerOne" and accept</t>
+  </si>
+  <si>
+    <t>Delete player name and accept</t>
+  </si>
+  <si>
+    <t>Delete player name and cancel</t>
+  </si>
+  <si>
+    <t>In Manage Name View delete "PlayerOne" and accept</t>
+  </si>
+  <si>
+    <t>In Manage Name View  delete"PlayerOne" and cancel</t>
+  </si>
+  <si>
+    <t>Player name "PlayerOne" is deleted, back to Player Selection View</t>
+  </si>
+  <si>
+    <t>Player name "PlayerOne" is not deleted,  back to Player Selection View</t>
+  </si>
+  <si>
+    <t>Scores and rankings are updated and displayed correctly before and after games in Result View and in Score Ranking in Home View</t>
   </si>
 </sst>
 </file>
@@ -113,7 +395,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,28 +427,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7644F5A8-28E0-439D-B11D-C996CBF9DCC1}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,189 +811,601 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-    </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="149.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="149.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="4" customFormat="1" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="4" customFormat="1" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="4" customFormat="1" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="4" customFormat="1" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="4" customFormat="1" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="4" customFormat="1" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="4" customFormat="1" ht="149.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="4" customFormat="1" ht="83.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D54" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="55" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D57" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="58" spans="1:4" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D61" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+    <row r="62" spans="1:4" s="4" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>